<commit_message>
Added and consilated all files from NK project to SDFQA by mkondapur
</commit_message>
<xml_diff>
--- a/target/classes/TestData/testDataSheet.xlsx
+++ b/target/classes/TestData/testDataSheet.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
@@ -51,7 +51,7 @@
     <t>test@gmail.com</t>
   </si>
   <si>
-    <t>Test123</t>
+    <t>Test1234</t>
   </si>
 </sst>
 </file>
@@ -464,7 +464,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>